<commit_message>
waiting for test: dynamic clause feature implemented.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoDbDynamicConditionStructure.xlsx
+++ b/meta/program/BlancoDbDynamicConditionStructure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbCommon/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C074B1-FF40-A94C-BD3F-8836A00706FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0897113-E39C-3543-AFF6-FA4908414975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19840" yWindow="460" windowWidth="18560" windowHeight="18800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,10 +263,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>dbCoumn</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>この動的条件句が対象とするitemを表すクラス</t>
     <rPh sb="2" eb="7">
       <t xml:space="preserve">ドウテキジョウケンク </t>
@@ -277,6 +273,10 @@
     <rPh sb="18" eb="19">
       <t xml:space="preserve">アラワス </t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>dbColumn</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -772,12 +772,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -785,12 +791,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:F36"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1204,12 +1204,12 @@
         <v>8</v>
       </c>
       <c r="B8" s="8"/>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="7" t="s">
@@ -1310,23 +1310,23 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="55"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="50"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="53"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="55"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
@@ -1363,29 +1363,29 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="55" t="s">
+      <c r="E25" s="50" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="50"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="29"/>
     </row>
     <row r="27" spans="1:6">
@@ -1439,10 +1439,10 @@
       <c r="D29" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="54" t="s">
+      <c r="E29" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="54"/>
+      <c r="F29" s="51"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="20">
@@ -1515,10 +1515,10 @@
       <c r="D33" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="54" t="s">
+      <c r="E33" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="54"/>
+      <c r="F33" s="51"/>
     </row>
     <row r="34" spans="1:6" ht="27.5" customHeight="1">
       <c r="A34" s="20">
@@ -1534,10 +1534,10 @@
       <c r="D34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="54" t="s">
+      <c r="E34" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="54"/>
+      <c r="F34" s="51"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="20">
@@ -1545,14 +1545,14 @@
         <v>9</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C35" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D35" s="34"/>
       <c r="E35" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F35" s="35"/>
     </row>
@@ -1561,16 +1561,16 @@
       <c r="B36" s="33"/>
       <c r="C36" s="34"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
     </row>
     <row r="37" spans="1:6" ht="32" customHeight="1">
       <c r="A37" s="20"/>
       <c r="B37" s="36"/>
       <c r="C37" s="37"/>
       <c r="D37" s="37"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="20"/>
@@ -1622,22 +1622,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="6">

</xml_diff>